<commit_message>
UPDATE ON MY CHECKS
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Sergio_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Sergio_v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
   <si>
     <t>2.1 Naming Conventions</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>44. Check that the implementation avoids \brutish programming": (see http://users.csc.calpoly.edu/~jdalbey/SWE/CodeSmells/bonehead.html).</t>
+  </si>
+  <si>
+    <t>OK?</t>
+  </si>
+  <si>
+    <t>N/A - comparison only with null</t>
   </si>
 </sst>
 </file>
@@ -381,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +412,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -419,11 +437,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -741,7 +761,7 @@
   <dimension ref="A1:A219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,27 +780,27 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -790,7 +810,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -800,7 +820,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -810,7 +830,7 @@
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -820,7 +840,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -830,7 +850,7 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -840,7 +860,7 @@
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -855,12 +875,12 @@
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -870,7 +890,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -885,7 +905,7 @@
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -895,7 +915,7 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -910,7 +930,7 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -920,7 +940,7 @@
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -930,7 +950,7 @@
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -945,7 +965,7 @@
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -955,7 +975,7 @@
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -965,7 +985,7 @@
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -980,7 +1000,7 @@
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -990,7 +1010,7 @@
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1005,7 +1025,7 @@
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1015,7 +1035,7 @@
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1024,11 +1044,19 @@
         <v>39</v>
       </c>
     </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+    </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>41</v>
@@ -1040,7 +1068,7 @@
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1049,354 +1077,477 @@
         <v>43</v>
       </c>
     </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>44</v>
+      <c r="A88" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>58</v>
+      <c r="A103" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A104" s="4" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A107" s="4" t="s">
         <v>62</v>
       </c>
     </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>63</v>
+      <c r="A110" s="5"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>64</v>
+      <c r="A113" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A114" s="5" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A117" s="4" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>68</v>
+      <c r="A120" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>69</v>
+      <c r="A123" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
-        <v>70</v>
+      <c r="A126" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>8</v>
+      <c r="A129" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>72</v>
+      <c r="A133" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A134" s="5" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
-        <v>75</v>
+      <c r="A137" s="5"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
-        <v>76</v>
+      <c r="A140" s="5"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>77</v>
+      <c r="A143" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
-        <v>78</v>
+      <c r="A144" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
-        <v>79</v>
+      <c r="A147" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
-        <v>80</v>
+      <c r="A150" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>81</v>
+      <c r="A153" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
-        <v>82</v>
+      <c r="A154" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>83</v>
+      <c r="A157" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
-        <v>84</v>
+      <c r="A158" s="5"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>85</v>
+      <c r="A161" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
-        <v>86</v>
+      <c r="A164" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>87</v>
+      <c r="A167" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
-        <v>113</v>
+      <c r="A168" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>8</v>
+      <c r="A171" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>8</v>
+      <c r="A174" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>8</v>
+      <c r="A177" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
-        <v>91</v>
+      <c r="A180" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
-        <v>92</v>
+      <c r="A183" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
-        <v>93</v>
+      <c r="A186" s="5"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="3" t="s">
-        <v>94</v>
+      <c r="A189" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>95</v>
+      <c r="A192" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
-        <v>96</v>
+      <c r="A193" s="5"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="3" t="s">
-        <v>97</v>
+      <c r="A196" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>98</v>
+      <c r="A199" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
-        <v>99</v>
+      <c r="A200" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="3" t="s">
-        <v>100</v>
+      <c r="A203" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="3" t="s">
-        <v>101</v>
+      <c r="A206" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>102</v>
+      <c r="A209" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="3" t="s">
-        <v>103</v>
+      <c r="A210" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
-        <v>104</v>
+      <c r="A213" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
-        <v>105</v>
+      <c r="A216" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
-        <v>106</v>
+      <c r="A219" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version of checks
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Sergio_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Sergio_v1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
   <si>
     <t>2.1 Naming Conventions</t>
   </si>
@@ -119,9 +119,6 @@
     <t>16. Higher-level breaks are used.</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>17. A new statement is aligned with the beginning of the expression at the same level as the previous line.</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>34. Check that parameters are presented in the correct order.</t>
   </si>
   <si>
-    <t>?? with respect to what?</t>
-  </si>
-  <si>
     <t>35. Check that the correct method is being called, or should it be a different method with a similar name.</t>
   </si>
   <si>
@@ -368,10 +362,25 @@
     <t>44. Check that the implementation avoids \brutish programming": (see http://users.csc.calpoly.edu/~jdalbey/SWE/CodeSmells/bonehead.html).</t>
   </si>
   <si>
-    <t>OK?</t>
-  </si>
-  <si>
     <t>N/A - comparison only with null</t>
+  </si>
+  <si>
+    <t>getPartyPaymentMethodValueMaps(Delegator, String)</t>
+  </si>
+  <si>
+    <t>getPaymentMethodAndRelated(ServletRequest, String)</t>
+  </si>
+  <si>
+    <t>getPaymentApplied(Delegator, String)</t>
+  </si>
+  <si>
+    <t>getPaymentAppliedAmount(Delegator, String)</t>
+  </si>
+  <si>
+    <t>getPaymentNotApplied(GenericValue, Boolean)</t>
+  </si>
+  <si>
+    <t>getPaymentNotApplied(Delegator, String)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,12 +427,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -437,13 +440,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -758,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A219"/>
+  <dimension ref="A1:A224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +778,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -806,7 +808,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -836,7 +838,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -846,7 +848,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -856,7 +858,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -975,28 +977,28 @@
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>31</v>
+      <c r="A57" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
@@ -1006,7 +1008,7 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
@@ -1016,12 +1018,12 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
@@ -1031,7 +1033,7 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
@@ -1041,7 +1043,7 @@
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
@@ -1051,20 +1053,22 @@
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
+      <c r="A80" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
@@ -1074,145 +1078,147 @@
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
+      <c r="A110" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>66</v>
+      <c r="A114" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
@@ -1222,7 +1228,7 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
@@ -1232,7 +1238,7 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
@@ -1242,7 +1248,7 @@
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
@@ -1252,301 +1258,336 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>74</v>
+      <c r="A134" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="5"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="5"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="5"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="5"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="5"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="4" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="4" t="s">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="3" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="4" t="s">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="4" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new file version + updates on excel (sergio+Soheil)
</commit_message>
<xml_diff>
--- a/5_CodeInspection/Code_checks_Sergio_v1.xlsx
+++ b/5_CodeInspection/Code_checks_Sergio_v1.xlsx
@@ -396,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +427,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -440,12 +446,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -762,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,32 +1284,32 @@
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="5" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>